<commit_message>
Start layout of motherboard
</commit_message>
<xml_diff>
--- a/2017/Motherboard/BOMs/Motherboard BOM.xlsx
+++ b/2017/Motherboard/BOMs/Motherboard BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>10uF Cap</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>MSOP8_3mmx3mm</t>
+  </si>
+  <si>
+    <t>Enclosure</t>
   </si>
 </sst>
 </file>
@@ -478,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +710,13 @@
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B21" s="2"/>
+      <c r="C21">
+        <v>14.66</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
@@ -735,6 +744,7 @@
     <hyperlink ref="A17" r:id="rId16"/>
     <hyperlink ref="A18" r:id="rId17"/>
     <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A21" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create and Finish ControlCard v1.0
The control board has 16 PWM outputs and 4 ADC inputs intended or
feedback
</commit_message>
<xml_diff>
--- a/2017/Motherboard/BOMs/Motherboard BOM.xlsx
+++ b/2017/Motherboard/BOMs/Motherboard BOM.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="4950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="4950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Power Budget" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>10uF Cap</t>
   </si>
@@ -114,13 +115,61 @@
   </si>
   <si>
     <t>Enclosure</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Total Current</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>3.3v</t>
+  </si>
+  <si>
+    <t>Current (mA)</t>
+  </si>
+  <si>
+    <t>Motherboard</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>1.5A Limit</t>
+  </si>
+  <si>
+    <t>PWM Board</t>
+  </si>
+  <si>
+    <t>PCA9685</t>
+  </si>
+  <si>
+    <t>Per pin, can sink 25mA and source 10mA</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>-40C to +85C</t>
+  </si>
+  <si>
+    <t>ADS1015</t>
+  </si>
+  <si>
+    <t>-40C to +125C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +181,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,12 +215,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,22 +568,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>603</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
+      <c r="A2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>805</v>
+        <v>603</v>
       </c>
       <c r="C3">
         <v>0.1</v>
@@ -532,10 +585,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -543,10 +596,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>805</v>
+        <v>603</v>
       </c>
       <c r="C5">
         <v>0.1</v>
@@ -554,7 +607,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2">
         <v>805</v>
@@ -565,35 +618,35 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C7">
-        <v>0.28999999999999998</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>603</v>
       </c>
       <c r="C8">
-        <v>0.27</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>603</v>
       </c>
       <c r="C9">
-        <v>2.5299999999999998</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -601,40 +654,40 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>0.78</v>
+        <v>2.5299999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C11">
-        <v>1.36</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2">
-        <v>805</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>1.36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>1206</v>
+        <v>805</v>
       </c>
       <c r="C13">
         <v>0.1</v>
@@ -642,10 +695,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="C14">
         <v>0.1</v>
@@ -653,99 +706,342 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>805</v>
       </c>
       <c r="C15">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>8.31</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>1.24</v>
+        <v>8.31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>0.98</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-    </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21">
+      <c r="B22" s="2"/>
+      <c r="C22">
         <v>14.66</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8" display="Femle DB9"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A16" r:id="rId14"/>
-    <hyperlink ref="A15" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A21" r:id="rId19"/>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="A9" r:id="rId7"/>
+    <hyperlink ref="A10" r:id="rId8" display="Femle DB9"/>
+    <hyperlink ref="A11" r:id="rId9"/>
+    <hyperlink ref="A12" r:id="rId10"/>
+    <hyperlink ref="A13" r:id="rId11"/>
+    <hyperlink ref="A14" r:id="rId12"/>
+    <hyperlink ref="A15" r:id="rId13"/>
+    <hyperlink ref="A17" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A18" r:id="rId16"/>
+    <hyperlink ref="A19" r:id="rId17"/>
+    <hyperlink ref="A20" r:id="rId18"/>
+    <hyperlink ref="A22" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="56.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="E3">
+        <f>B3*D3</f>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>0.05</v>
+      </c>
+      <c r="E4">
+        <f>B4*D4</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>3.84</v>
+      </c>
+      <c r="E5">
+        <f>B5*D5</f>
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <f>B8*D8</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>200</v>
+      </c>
+      <c r="E11">
+        <f>B11*D11</f>
+        <v>200</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
+        <v>0.15</v>
+      </c>
+      <c r="E12">
+        <f>B12*D12</f>
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="A11" r:id="rId7"/>
+    <hyperlink ref="A12" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+</worksheet>
 </file>
</xml_diff>